<commit_message>
Update data files, improve file loading processes and refactory in StockEnv
</commit_message>
<xml_diff>
--- a/Env/stock_data/1101/2016.xlsx
+++ b/Env/stock_data/1101/2016.xlsx
@@ -831,7 +831,7 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>20160201</v>
@@ -851,7 +851,7 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>20160202</v>
@@ -871,7 +871,7 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>20160203</v>
@@ -891,7 +891,7 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>20160215</v>
@@ -911,7 +911,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>20160216</v>
@@ -931,7 +931,7 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>20160217</v>
@@ -951,7 +951,7 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>20160218</v>
@@ -971,7 +971,7 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>20160219</v>
@@ -991,7 +991,7 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <v>20160222</v>
@@ -1011,7 +1011,7 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <v>20160223</v>
@@ -1031,7 +1031,7 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>20160224</v>
@@ -1051,7 +1051,7 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B34">
         <v>20160225</v>
@@ -1071,7 +1071,7 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <v>20160226</v>
@@ -1091,7 +1091,7 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="1">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B36">
         <v>20160301</v>
@@ -1111,7 +1111,7 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="1">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <v>20160302</v>
@@ -1131,7 +1131,7 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="1">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <v>20160303</v>
@@ -1151,7 +1151,7 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="1">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="B39">
         <v>20160304</v>
@@ -1171,7 +1171,7 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <v>20160307</v>
@@ -1191,7 +1191,7 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B41">
         <v>20160308</v>
@@ -1211,7 +1211,7 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="1">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B42">
         <v>20160309</v>
@@ -1231,7 +1231,7 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="1">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B43">
         <v>20160310</v>
@@ -1251,7 +1251,7 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="1">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B44">
         <v>20160311</v>
@@ -1271,7 +1271,7 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="1">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="B45">
         <v>20160314</v>
@@ -1291,7 +1291,7 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="1">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="B46">
         <v>20160315</v>
@@ -1311,7 +1311,7 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="1">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="B47">
         <v>20160316</v>
@@ -1331,7 +1331,7 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="1">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="B48">
         <v>20160317</v>
@@ -1351,7 +1351,7 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="1">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="B49">
         <v>20160318</v>
@@ -1371,7 +1371,7 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="1">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="B50">
         <v>20160321</v>
@@ -1391,7 +1391,7 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="1">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="B51">
         <v>20160322</v>
@@ -1411,7 +1411,7 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="1">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="B52">
         <v>20160323</v>
@@ -1431,7 +1431,7 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="1">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="B53">
         <v>20160324</v>
@@ -1451,7 +1451,7 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="1">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="B54">
         <v>20160325</v>
@@ -1471,7 +1471,7 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="1">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B55">
         <v>20160328</v>
@@ -1491,7 +1491,7 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="1">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="B56">
         <v>20160329</v>
@@ -1511,7 +1511,7 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="1">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="B57">
         <v>20160330</v>
@@ -1531,7 +1531,7 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="1">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="B58">
         <v>20160331</v>
@@ -1551,7 +1551,7 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="1">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="B59">
         <v>20160401</v>
@@ -1571,7 +1571,7 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="1">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="B60">
         <v>20160406</v>
@@ -1591,7 +1591,7 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="1">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="B61">
         <v>20160407</v>
@@ -1611,7 +1611,7 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="1">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="B62">
         <v>20160408</v>
@@ -1631,7 +1631,7 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="1">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="B63">
         <v>20160411</v>
@@ -1651,7 +1651,7 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="1">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="B64">
         <v>20160412</v>
@@ -1671,7 +1671,7 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="1">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="B65">
         <v>20160413</v>
@@ -1691,7 +1691,7 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="1">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="B66">
         <v>20160414</v>
@@ -1711,7 +1711,7 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="1">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="B67">
         <v>20160415</v>
@@ -1731,7 +1731,7 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="1">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="B68">
         <v>20160418</v>
@@ -1751,7 +1751,7 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="1">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="B69">
         <v>20160419</v>
@@ -1771,7 +1771,7 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="1">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="B70">
         <v>20160420</v>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="1">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B71">
         <v>20160421</v>
@@ -1811,7 +1811,7 @@
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="1">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="B72">
         <v>20160422</v>
@@ -1831,7 +1831,7 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="1">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="B73">
         <v>20160425</v>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="1">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="B74">
         <v>20160426</v>
@@ -1871,7 +1871,7 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="1">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="B75">
         <v>20160427</v>
@@ -1891,7 +1891,7 @@
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="1">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="B76">
         <v>20160428</v>
@@ -1911,7 +1911,7 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="1">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="B77">
         <v>20160429</v>
@@ -1931,7 +1931,7 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="1">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="B78">
         <v>20160503</v>
@@ -1951,7 +1951,7 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="1">
-        <v>1</v>
+        <v>77</v>
       </c>
       <c r="B79">
         <v>20160504</v>
@@ -1971,7 +1971,7 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="1">
-        <v>2</v>
+        <v>78</v>
       </c>
       <c r="B80">
         <v>20160505</v>
@@ -1991,7 +1991,7 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="1">
-        <v>3</v>
+        <v>79</v>
       </c>
       <c r="B81">
         <v>20160506</v>
@@ -2011,7 +2011,7 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="1">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="B82">
         <v>20160509</v>
@@ -2031,7 +2031,7 @@
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="1">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="B83">
         <v>20160510</v>
@@ -2051,7 +2051,7 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="1">
-        <v>6</v>
+        <v>82</v>
       </c>
       <c r="B84">
         <v>20160511</v>
@@ -2071,7 +2071,7 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="1">
-        <v>7</v>
+        <v>83</v>
       </c>
       <c r="B85">
         <v>20160512</v>
@@ -2091,7 +2091,7 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="1">
-        <v>8</v>
+        <v>84</v>
       </c>
       <c r="B86">
         <v>20160513</v>
@@ -2111,7 +2111,7 @@
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="1">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="B87">
         <v>20160516</v>
@@ -2131,7 +2131,7 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="1">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="B88">
         <v>20160517</v>
@@ -2151,7 +2151,7 @@
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="1">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="B89">
         <v>20160518</v>
@@ -2171,7 +2171,7 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="1">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="B90">
         <v>20160519</v>
@@ -2191,7 +2191,7 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="1">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="B91">
         <v>20160520</v>
@@ -2211,7 +2211,7 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="1">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="B92">
         <v>20160523</v>
@@ -2231,7 +2231,7 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="1">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="B93">
         <v>20160524</v>
@@ -2251,7 +2251,7 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="1">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="B94">
         <v>20160525</v>
@@ -2271,7 +2271,7 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="1">
-        <v>17</v>
+        <v>93</v>
       </c>
       <c r="B95">
         <v>20160526</v>
@@ -2291,7 +2291,7 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="1">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="B96">
         <v>20160527</v>
@@ -2311,7 +2311,7 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="1">
-        <v>19</v>
+        <v>95</v>
       </c>
       <c r="B97">
         <v>20160530</v>
@@ -2331,7 +2331,7 @@
     </row>
     <row r="98" spans="1:6">
       <c r="A98" s="1">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="B98">
         <v>20160531</v>
@@ -2351,7 +2351,7 @@
     </row>
     <row r="99" spans="1:6">
       <c r="A99" s="1">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="B99">
         <v>20160601</v>
@@ -2371,7 +2371,7 @@
     </row>
     <row r="100" spans="1:6">
       <c r="A100" s="1">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="B100">
         <v>20160602</v>
@@ -2391,7 +2391,7 @@
     </row>
     <row r="101" spans="1:6">
       <c r="A101" s="1">
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="B101">
         <v>20160603</v>
@@ -2411,7 +2411,7 @@
     </row>
     <row r="102" spans="1:6">
       <c r="A102" s="1">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="B102">
         <v>20160604</v>
@@ -2431,7 +2431,7 @@
     </row>
     <row r="103" spans="1:6">
       <c r="A103" s="1">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="B103">
         <v>20160606</v>
@@ -2451,7 +2451,7 @@
     </row>
     <row r="104" spans="1:6">
       <c r="A104" s="1">
-        <v>5</v>
+        <v>102</v>
       </c>
       <c r="B104">
         <v>20160607</v>
@@ -2471,7 +2471,7 @@
     </row>
     <row r="105" spans="1:6">
       <c r="A105" s="1">
-        <v>6</v>
+        <v>103</v>
       </c>
       <c r="B105">
         <v>20160608</v>
@@ -2491,7 +2491,7 @@
     </row>
     <row r="106" spans="1:6">
       <c r="A106" s="1">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="B106">
         <v>20160613</v>
@@ -2511,7 +2511,7 @@
     </row>
     <row r="107" spans="1:6">
       <c r="A107" s="1">
-        <v>8</v>
+        <v>105</v>
       </c>
       <c r="B107">
         <v>20160614</v>
@@ -2531,7 +2531,7 @@
     </row>
     <row r="108" spans="1:6">
       <c r="A108" s="1">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="B108">
         <v>20160615</v>
@@ -2551,7 +2551,7 @@
     </row>
     <row r="109" spans="1:6">
       <c r="A109" s="1">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="B109">
         <v>20160616</v>
@@ -2571,7 +2571,7 @@
     </row>
     <row r="110" spans="1:6">
       <c r="A110" s="1">
-        <v>11</v>
+        <v>108</v>
       </c>
       <c r="B110">
         <v>20160617</v>
@@ -2591,7 +2591,7 @@
     </row>
     <row r="111" spans="1:6">
       <c r="A111" s="1">
-        <v>12</v>
+        <v>109</v>
       </c>
       <c r="B111">
         <v>20160620</v>
@@ -2611,7 +2611,7 @@
     </row>
     <row r="112" spans="1:6">
       <c r="A112" s="1">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="B112">
         <v>20160621</v>
@@ -2631,7 +2631,7 @@
     </row>
     <row r="113" spans="1:6">
       <c r="A113" s="1">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="B113">
         <v>20160622</v>
@@ -2651,7 +2651,7 @@
     </row>
     <row r="114" spans="1:6">
       <c r="A114" s="1">
-        <v>15</v>
+        <v>112</v>
       </c>
       <c r="B114">
         <v>20160623</v>
@@ -2671,7 +2671,7 @@
     </row>
     <row r="115" spans="1:6">
       <c r="A115" s="1">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="B115">
         <v>20160624</v>
@@ -2691,7 +2691,7 @@
     </row>
     <row r="116" spans="1:6">
       <c r="A116" s="1">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="B116">
         <v>20160627</v>
@@ -2711,7 +2711,7 @@
     </row>
     <row r="117" spans="1:6">
       <c r="A117" s="1">
-        <v>18</v>
+        <v>115</v>
       </c>
       <c r="B117">
         <v>20160628</v>
@@ -2731,7 +2731,7 @@
     </row>
     <row r="118" spans="1:6">
       <c r="A118" s="1">
-        <v>19</v>
+        <v>116</v>
       </c>
       <c r="B118">
         <v>20160629</v>
@@ -2751,7 +2751,7 @@
     </row>
     <row r="119" spans="1:6">
       <c r="A119" s="1">
-        <v>20</v>
+        <v>117</v>
       </c>
       <c r="B119">
         <v>20160630</v>
@@ -2771,7 +2771,7 @@
     </row>
     <row r="120" spans="1:6">
       <c r="A120" s="1">
-        <v>0</v>
+        <v>118</v>
       </c>
       <c r="B120">
         <v>20160701</v>
@@ -2791,7 +2791,7 @@
     </row>
     <row r="121" spans="1:6">
       <c r="A121" s="1">
-        <v>1</v>
+        <v>119</v>
       </c>
       <c r="B121">
         <v>20160704</v>
@@ -2811,7 +2811,7 @@
     </row>
     <row r="122" spans="1:6">
       <c r="A122" s="1">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="B122">
         <v>20160705</v>
@@ -2831,7 +2831,7 @@
     </row>
     <row r="123" spans="1:6">
       <c r="A123" s="1">
-        <v>3</v>
+        <v>121</v>
       </c>
       <c r="B123">
         <v>20160706</v>
@@ -2851,7 +2851,7 @@
     </row>
     <row r="124" spans="1:6">
       <c r="A124" s="1">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="B124">
         <v>20160707</v>
@@ -2871,7 +2871,7 @@
     </row>
     <row r="125" spans="1:6">
       <c r="A125" s="1">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="B125">
         <v>20160711</v>
@@ -2891,7 +2891,7 @@
     </row>
     <row r="126" spans="1:6">
       <c r="A126" s="1">
-        <v>6</v>
+        <v>124</v>
       </c>
       <c r="B126">
         <v>20160712</v>
@@ -2911,7 +2911,7 @@
     </row>
     <row r="127" spans="1:6">
       <c r="A127" s="1">
-        <v>7</v>
+        <v>125</v>
       </c>
       <c r="B127">
         <v>20160713</v>
@@ -2931,7 +2931,7 @@
     </row>
     <row r="128" spans="1:6">
       <c r="A128" s="1">
-        <v>8</v>
+        <v>126</v>
       </c>
       <c r="B128">
         <v>20160714</v>
@@ -2951,7 +2951,7 @@
     </row>
     <row r="129" spans="1:6">
       <c r="A129" s="1">
-        <v>9</v>
+        <v>127</v>
       </c>
       <c r="B129">
         <v>20160715</v>
@@ -2971,7 +2971,7 @@
     </row>
     <row r="130" spans="1:6">
       <c r="A130" s="1">
-        <v>10</v>
+        <v>128</v>
       </c>
       <c r="B130">
         <v>20160718</v>
@@ -2991,7 +2991,7 @@
     </row>
     <row r="131" spans="1:6">
       <c r="A131" s="1">
-        <v>11</v>
+        <v>129</v>
       </c>
       <c r="B131">
         <v>20160719</v>
@@ -3011,7 +3011,7 @@
     </row>
     <row r="132" spans="1:6">
       <c r="A132" s="1">
-        <v>12</v>
+        <v>130</v>
       </c>
       <c r="B132">
         <v>20160720</v>
@@ -3031,7 +3031,7 @@
     </row>
     <row r="133" spans="1:6">
       <c r="A133" s="1">
-        <v>13</v>
+        <v>131</v>
       </c>
       <c r="B133">
         <v>20160721</v>
@@ -3051,7 +3051,7 @@
     </row>
     <row r="134" spans="1:6">
       <c r="A134" s="1">
-        <v>14</v>
+        <v>132</v>
       </c>
       <c r="B134">
         <v>20160722</v>
@@ -3071,7 +3071,7 @@
     </row>
     <row r="135" spans="1:6">
       <c r="A135" s="1">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="B135">
         <v>20160725</v>
@@ -3091,7 +3091,7 @@
     </row>
     <row r="136" spans="1:6">
       <c r="A136" s="1">
-        <v>16</v>
+        <v>134</v>
       </c>
       <c r="B136">
         <v>20160726</v>
@@ -3111,7 +3111,7 @@
     </row>
     <row r="137" spans="1:6">
       <c r="A137" s="1">
-        <v>17</v>
+        <v>135</v>
       </c>
       <c r="B137">
         <v>20160727</v>
@@ -3131,7 +3131,7 @@
     </row>
     <row r="138" spans="1:6">
       <c r="A138" s="1">
-        <v>18</v>
+        <v>136</v>
       </c>
       <c r="B138">
         <v>20160728</v>
@@ -3151,7 +3151,7 @@
     </row>
     <row r="139" spans="1:6">
       <c r="A139" s="1">
-        <v>19</v>
+        <v>137</v>
       </c>
       <c r="B139">
         <v>20160729</v>
@@ -3171,7 +3171,7 @@
     </row>
     <row r="140" spans="1:6">
       <c r="A140" s="1">
-        <v>0</v>
+        <v>138</v>
       </c>
       <c r="B140">
         <v>20160801</v>
@@ -3191,7 +3191,7 @@
     </row>
     <row r="141" spans="1:6">
       <c r="A141" s="1">
-        <v>1</v>
+        <v>139</v>
       </c>
       <c r="B141">
         <v>20160802</v>
@@ -3211,7 +3211,7 @@
     </row>
     <row r="142" spans="1:6">
       <c r="A142" s="1">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="B142">
         <v>20160803</v>
@@ -3231,7 +3231,7 @@
     </row>
     <row r="143" spans="1:6">
       <c r="A143" s="1">
-        <v>3</v>
+        <v>141</v>
       </c>
       <c r="B143">
         <v>20160804</v>
@@ -3251,7 +3251,7 @@
     </row>
     <row r="144" spans="1:6">
       <c r="A144" s="1">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="B144">
         <v>20160805</v>
@@ -3271,7 +3271,7 @@
     </row>
     <row r="145" spans="1:6">
       <c r="A145" s="1">
-        <v>5</v>
+        <v>143</v>
       </c>
       <c r="B145">
         <v>20160808</v>
@@ -3291,7 +3291,7 @@
     </row>
     <row r="146" spans="1:6">
       <c r="A146" s="1">
-        <v>6</v>
+        <v>144</v>
       </c>
       <c r="B146">
         <v>20160809</v>
@@ -3311,7 +3311,7 @@
     </row>
     <row r="147" spans="1:6">
       <c r="A147" s="1">
-        <v>7</v>
+        <v>145</v>
       </c>
       <c r="B147">
         <v>20160810</v>
@@ -3331,7 +3331,7 @@
     </row>
     <row r="148" spans="1:6">
       <c r="A148" s="1">
-        <v>8</v>
+        <v>146</v>
       </c>
       <c r="B148">
         <v>20160811</v>
@@ -3351,7 +3351,7 @@
     </row>
     <row r="149" spans="1:6">
       <c r="A149" s="1">
-        <v>9</v>
+        <v>147</v>
       </c>
       <c r="B149">
         <v>20160812</v>
@@ -3371,7 +3371,7 @@
     </row>
     <row r="150" spans="1:6">
       <c r="A150" s="1">
-        <v>10</v>
+        <v>148</v>
       </c>
       <c r="B150">
         <v>20160815</v>
@@ -3391,7 +3391,7 @@
     </row>
     <row r="151" spans="1:6">
       <c r="A151" s="1">
-        <v>11</v>
+        <v>149</v>
       </c>
       <c r="B151">
         <v>20160816</v>
@@ -3411,7 +3411,7 @@
     </row>
     <row r="152" spans="1:6">
       <c r="A152" s="1">
-        <v>12</v>
+        <v>150</v>
       </c>
       <c r="B152">
         <v>20160817</v>
@@ -3431,7 +3431,7 @@
     </row>
     <row r="153" spans="1:6">
       <c r="A153" s="1">
-        <v>13</v>
+        <v>151</v>
       </c>
       <c r="B153">
         <v>20160818</v>
@@ -3451,7 +3451,7 @@
     </row>
     <row r="154" spans="1:6">
       <c r="A154" s="1">
-        <v>14</v>
+        <v>152</v>
       </c>
       <c r="B154">
         <v>20160819</v>
@@ -3471,7 +3471,7 @@
     </row>
     <row r="155" spans="1:6">
       <c r="A155" s="1">
-        <v>15</v>
+        <v>153</v>
       </c>
       <c r="B155">
         <v>20160822</v>
@@ -3491,7 +3491,7 @@
     </row>
     <row r="156" spans="1:6">
       <c r="A156" s="1">
-        <v>16</v>
+        <v>154</v>
       </c>
       <c r="B156">
         <v>20160823</v>
@@ -3511,7 +3511,7 @@
     </row>
     <row r="157" spans="1:6">
       <c r="A157" s="1">
-        <v>17</v>
+        <v>155</v>
       </c>
       <c r="B157">
         <v>20160824</v>
@@ -3531,7 +3531,7 @@
     </row>
     <row r="158" spans="1:6">
       <c r="A158" s="1">
-        <v>18</v>
+        <v>156</v>
       </c>
       <c r="B158">
         <v>20160825</v>
@@ -3551,7 +3551,7 @@
     </row>
     <row r="159" spans="1:6">
       <c r="A159" s="1">
-        <v>19</v>
+        <v>157</v>
       </c>
       <c r="B159">
         <v>20160826</v>
@@ -3571,7 +3571,7 @@
     </row>
     <row r="160" spans="1:6">
       <c r="A160" s="1">
-        <v>20</v>
+        <v>158</v>
       </c>
       <c r="B160">
         <v>20160829</v>
@@ -3591,7 +3591,7 @@
     </row>
     <row r="161" spans="1:6">
       <c r="A161" s="1">
-        <v>21</v>
+        <v>159</v>
       </c>
       <c r="B161">
         <v>20160830</v>
@@ -3611,7 +3611,7 @@
     </row>
     <row r="162" spans="1:6">
       <c r="A162" s="1">
-        <v>22</v>
+        <v>160</v>
       </c>
       <c r="B162">
         <v>20160831</v>
@@ -3631,7 +3631,7 @@
     </row>
     <row r="163" spans="1:6">
       <c r="A163" s="1">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="B163">
         <v>20160901</v>
@@ -3651,7 +3651,7 @@
     </row>
     <row r="164" spans="1:6">
       <c r="A164" s="1">
-        <v>1</v>
+        <v>162</v>
       </c>
       <c r="B164">
         <v>20160902</v>
@@ -3671,7 +3671,7 @@
     </row>
     <row r="165" spans="1:6">
       <c r="A165" s="1">
-        <v>2</v>
+        <v>163</v>
       </c>
       <c r="B165">
         <v>20160905</v>
@@ -3691,7 +3691,7 @@
     </row>
     <row r="166" spans="1:6">
       <c r="A166" s="1">
-        <v>3</v>
+        <v>164</v>
       </c>
       <c r="B166">
         <v>20160906</v>
@@ -3711,7 +3711,7 @@
     </row>
     <row r="167" spans="1:6">
       <c r="A167" s="1">
-        <v>4</v>
+        <v>165</v>
       </c>
       <c r="B167">
         <v>20160907</v>
@@ -3731,7 +3731,7 @@
     </row>
     <row r="168" spans="1:6">
       <c r="A168" s="1">
-        <v>5</v>
+        <v>166</v>
       </c>
       <c r="B168">
         <v>20160908</v>
@@ -3751,7 +3751,7 @@
     </row>
     <row r="169" spans="1:6">
       <c r="A169" s="1">
-        <v>6</v>
+        <v>167</v>
       </c>
       <c r="B169">
         <v>20160909</v>
@@ -3771,7 +3771,7 @@
     </row>
     <row r="170" spans="1:6">
       <c r="A170" s="1">
-        <v>7</v>
+        <v>168</v>
       </c>
       <c r="B170">
         <v>20160910</v>
@@ -3791,7 +3791,7 @@
     </row>
     <row r="171" spans="1:6">
       <c r="A171" s="1">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="B171">
         <v>20160912</v>
@@ -3811,7 +3811,7 @@
     </row>
     <row r="172" spans="1:6">
       <c r="A172" s="1">
-        <v>9</v>
+        <v>170</v>
       </c>
       <c r="B172">
         <v>20160913</v>
@@ -3831,7 +3831,7 @@
     </row>
     <row r="173" spans="1:6">
       <c r="A173" s="1">
-        <v>10</v>
+        <v>171</v>
       </c>
       <c r="B173">
         <v>20160914</v>
@@ -3851,7 +3851,7 @@
     </row>
     <row r="174" spans="1:6">
       <c r="A174" s="1">
-        <v>11</v>
+        <v>172</v>
       </c>
       <c r="B174">
         <v>20160919</v>
@@ -3871,7 +3871,7 @@
     </row>
     <row r="175" spans="1:6">
       <c r="A175" s="1">
-        <v>12</v>
+        <v>173</v>
       </c>
       <c r="B175">
         <v>20160920</v>
@@ -3891,7 +3891,7 @@
     </row>
     <row r="176" spans="1:6">
       <c r="A176" s="1">
-        <v>13</v>
+        <v>174</v>
       </c>
       <c r="B176">
         <v>20160921</v>
@@ -3911,7 +3911,7 @@
     </row>
     <row r="177" spans="1:6">
       <c r="A177" s="1">
-        <v>14</v>
+        <v>175</v>
       </c>
       <c r="B177">
         <v>20160922</v>
@@ -3931,7 +3931,7 @@
     </row>
     <row r="178" spans="1:6">
       <c r="A178" s="1">
-        <v>15</v>
+        <v>176</v>
       </c>
       <c r="B178">
         <v>20160923</v>
@@ -3951,7 +3951,7 @@
     </row>
     <row r="179" spans="1:6">
       <c r="A179" s="1">
-        <v>16</v>
+        <v>177</v>
       </c>
       <c r="B179">
         <v>20160926</v>
@@ -3971,7 +3971,7 @@
     </row>
     <row r="180" spans="1:6">
       <c r="A180" s="1">
-        <v>17</v>
+        <v>178</v>
       </c>
       <c r="B180">
         <v>20160929</v>
@@ -3991,7 +3991,7 @@
     </row>
     <row r="181" spans="1:6">
       <c r="A181" s="1">
-        <v>18</v>
+        <v>179</v>
       </c>
       <c r="B181">
         <v>20160930</v>
@@ -4011,7 +4011,7 @@
     </row>
     <row r="182" spans="1:6">
       <c r="A182" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="B182">
         <v>20161003</v>
@@ -4031,7 +4031,7 @@
     </row>
     <row r="183" spans="1:6">
       <c r="A183" s="1">
-        <v>1</v>
+        <v>181</v>
       </c>
       <c r="B183">
         <v>20161004</v>
@@ -4051,7 +4051,7 @@
     </row>
     <row r="184" spans="1:6">
       <c r="A184" s="1">
-        <v>2</v>
+        <v>182</v>
       </c>
       <c r="B184">
         <v>20161005</v>
@@ -4071,7 +4071,7 @@
     </row>
     <row r="185" spans="1:6">
       <c r="A185" s="1">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="B185">
         <v>20161006</v>
@@ -4091,7 +4091,7 @@
     </row>
     <row r="186" spans="1:6">
       <c r="A186" s="1">
-        <v>4</v>
+        <v>184</v>
       </c>
       <c r="B186">
         <v>20161007</v>
@@ -4111,7 +4111,7 @@
     </row>
     <row r="187" spans="1:6">
       <c r="A187" s="1">
-        <v>5</v>
+        <v>185</v>
       </c>
       <c r="B187">
         <v>20161011</v>
@@ -4131,7 +4131,7 @@
     </row>
     <row r="188" spans="1:6">
       <c r="A188" s="1">
-        <v>6</v>
+        <v>186</v>
       </c>
       <c r="B188">
         <v>20161012</v>
@@ -4151,7 +4151,7 @@
     </row>
     <row r="189" spans="1:6">
       <c r="A189" s="1">
-        <v>7</v>
+        <v>187</v>
       </c>
       <c r="B189">
         <v>20161013</v>
@@ -4171,7 +4171,7 @@
     </row>
     <row r="190" spans="1:6">
       <c r="A190" s="1">
-        <v>8</v>
+        <v>188</v>
       </c>
       <c r="B190">
         <v>20161014</v>
@@ -4191,7 +4191,7 @@
     </row>
     <row r="191" spans="1:6">
       <c r="A191" s="1">
-        <v>9</v>
+        <v>189</v>
       </c>
       <c r="B191">
         <v>20161017</v>
@@ -4211,7 +4211,7 @@
     </row>
     <row r="192" spans="1:6">
       <c r="A192" s="1">
-        <v>10</v>
+        <v>190</v>
       </c>
       <c r="B192">
         <v>20161018</v>
@@ -4231,7 +4231,7 @@
     </row>
     <row r="193" spans="1:6">
       <c r="A193" s="1">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="B193">
         <v>20161019</v>
@@ -4251,7 +4251,7 @@
     </row>
     <row r="194" spans="1:6">
       <c r="A194" s="1">
-        <v>12</v>
+        <v>192</v>
       </c>
       <c r="B194">
         <v>20161020</v>
@@ -4271,7 +4271,7 @@
     </row>
     <row r="195" spans="1:6">
       <c r="A195" s="1">
-        <v>13</v>
+        <v>193</v>
       </c>
       <c r="B195">
         <v>20161021</v>
@@ -4291,7 +4291,7 @@
     </row>
     <row r="196" spans="1:6">
       <c r="A196" s="1">
-        <v>14</v>
+        <v>194</v>
       </c>
       <c r="B196">
         <v>20161024</v>
@@ -4311,7 +4311,7 @@
     </row>
     <row r="197" spans="1:6">
       <c r="A197" s="1">
-        <v>15</v>
+        <v>195</v>
       </c>
       <c r="B197">
         <v>20161025</v>
@@ -4331,7 +4331,7 @@
     </row>
     <row r="198" spans="1:6">
       <c r="A198" s="1">
-        <v>16</v>
+        <v>196</v>
       </c>
       <c r="B198">
         <v>20161026</v>
@@ -4351,7 +4351,7 @@
     </row>
     <row r="199" spans="1:6">
       <c r="A199" s="1">
-        <v>17</v>
+        <v>197</v>
       </c>
       <c r="B199">
         <v>20161027</v>
@@ -4371,7 +4371,7 @@
     </row>
     <row r="200" spans="1:6">
       <c r="A200" s="1">
-        <v>18</v>
+        <v>198</v>
       </c>
       <c r="B200">
         <v>20161028</v>
@@ -4391,7 +4391,7 @@
     </row>
     <row r="201" spans="1:6">
       <c r="A201" s="1">
-        <v>19</v>
+        <v>199</v>
       </c>
       <c r="B201">
         <v>20161031</v>
@@ -4411,7 +4411,7 @@
     </row>
     <row r="202" spans="1:6">
       <c r="A202" s="1">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="B202">
         <v>20161101</v>
@@ -4431,7 +4431,7 @@
     </row>
     <row r="203" spans="1:6">
       <c r="A203" s="1">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="B203">
         <v>20161102</v>
@@ -4451,7 +4451,7 @@
     </row>
     <row r="204" spans="1:6">
       <c r="A204" s="1">
-        <v>2</v>
+        <v>202</v>
       </c>
       <c r="B204">
         <v>20161103</v>
@@ -4471,7 +4471,7 @@
     </row>
     <row r="205" spans="1:6">
       <c r="A205" s="1">
-        <v>3</v>
+        <v>203</v>
       </c>
       <c r="B205">
         <v>20161104</v>
@@ -4491,7 +4491,7 @@
     </row>
     <row r="206" spans="1:6">
       <c r="A206" s="1">
-        <v>4</v>
+        <v>204</v>
       </c>
       <c r="B206">
         <v>20161107</v>
@@ -4511,7 +4511,7 @@
     </row>
     <row r="207" spans="1:6">
       <c r="A207" s="1">
-        <v>5</v>
+        <v>205</v>
       </c>
       <c r="B207">
         <v>20161108</v>
@@ -4531,7 +4531,7 @@
     </row>
     <row r="208" spans="1:6">
       <c r="A208" s="1">
-        <v>6</v>
+        <v>206</v>
       </c>
       <c r="B208">
         <v>20161109</v>
@@ -4551,7 +4551,7 @@
     </row>
     <row r="209" spans="1:6">
       <c r="A209" s="1">
-        <v>7</v>
+        <v>207</v>
       </c>
       <c r="B209">
         <v>20161110</v>
@@ -4571,7 +4571,7 @@
     </row>
     <row r="210" spans="1:6">
       <c r="A210" s="1">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="B210">
         <v>20161111</v>
@@ -4591,7 +4591,7 @@
     </row>
     <row r="211" spans="1:6">
       <c r="A211" s="1">
-        <v>9</v>
+        <v>209</v>
       </c>
       <c r="B211">
         <v>20161114</v>
@@ -4611,7 +4611,7 @@
     </row>
     <row r="212" spans="1:6">
       <c r="A212" s="1">
-        <v>10</v>
+        <v>210</v>
       </c>
       <c r="B212">
         <v>20161115</v>
@@ -4631,7 +4631,7 @@
     </row>
     <row r="213" spans="1:6">
       <c r="A213" s="1">
-        <v>11</v>
+        <v>211</v>
       </c>
       <c r="B213">
         <v>20161116</v>
@@ -4651,7 +4651,7 @@
     </row>
     <row r="214" spans="1:6">
       <c r="A214" s="1">
-        <v>12</v>
+        <v>212</v>
       </c>
       <c r="B214">
         <v>20161117</v>
@@ -4671,7 +4671,7 @@
     </row>
     <row r="215" spans="1:6">
       <c r="A215" s="1">
-        <v>13</v>
+        <v>213</v>
       </c>
       <c r="B215">
         <v>20161118</v>
@@ -4691,7 +4691,7 @@
     </row>
     <row r="216" spans="1:6">
       <c r="A216" s="1">
-        <v>14</v>
+        <v>214</v>
       </c>
       <c r="B216">
         <v>20161121</v>
@@ -4711,7 +4711,7 @@
     </row>
     <row r="217" spans="1:6">
       <c r="A217" s="1">
-        <v>15</v>
+        <v>215</v>
       </c>
       <c r="B217">
         <v>20161122</v>
@@ -4731,7 +4731,7 @@
     </row>
     <row r="218" spans="1:6">
       <c r="A218" s="1">
-        <v>16</v>
+        <v>216</v>
       </c>
       <c r="B218">
         <v>20161123</v>
@@ -4751,7 +4751,7 @@
     </row>
     <row r="219" spans="1:6">
       <c r="A219" s="1">
-        <v>17</v>
+        <v>217</v>
       </c>
       <c r="B219">
         <v>20161124</v>
@@ -4771,7 +4771,7 @@
     </row>
     <row r="220" spans="1:6">
       <c r="A220" s="1">
-        <v>18</v>
+        <v>218</v>
       </c>
       <c r="B220">
         <v>20161125</v>
@@ -4791,7 +4791,7 @@
     </row>
     <row r="221" spans="1:6">
       <c r="A221" s="1">
-        <v>19</v>
+        <v>219</v>
       </c>
       <c r="B221">
         <v>20161128</v>
@@ -4811,7 +4811,7 @@
     </row>
     <row r="222" spans="1:6">
       <c r="A222" s="1">
-        <v>20</v>
+        <v>220</v>
       </c>
       <c r="B222">
         <v>20161129</v>
@@ -4831,7 +4831,7 @@
     </row>
     <row r="223" spans="1:6">
       <c r="A223" s="1">
-        <v>21</v>
+        <v>221</v>
       </c>
       <c r="B223">
         <v>20161130</v>
@@ -4851,7 +4851,7 @@
     </row>
     <row r="224" spans="1:6">
       <c r="A224" s="1">
-        <v>0</v>
+        <v>222</v>
       </c>
       <c r="B224">
         <v>20161201</v>
@@ -4871,7 +4871,7 @@
     </row>
     <row r="225" spans="1:6">
       <c r="A225" s="1">
-        <v>1</v>
+        <v>223</v>
       </c>
       <c r="B225">
         <v>20161202</v>
@@ -4891,7 +4891,7 @@
     </row>
     <row r="226" spans="1:6">
       <c r="A226" s="1">
-        <v>2</v>
+        <v>224</v>
       </c>
       <c r="B226">
         <v>20161205</v>
@@ -4911,7 +4911,7 @@
     </row>
     <row r="227" spans="1:6">
       <c r="A227" s="1">
-        <v>3</v>
+        <v>225</v>
       </c>
       <c r="B227">
         <v>20161206</v>
@@ -4931,7 +4931,7 @@
     </row>
     <row r="228" spans="1:6">
       <c r="A228" s="1">
-        <v>4</v>
+        <v>226</v>
       </c>
       <c r="B228">
         <v>20161207</v>
@@ -4951,7 +4951,7 @@
     </row>
     <row r="229" spans="1:6">
       <c r="A229" s="1">
-        <v>5</v>
+        <v>227</v>
       </c>
       <c r="B229">
         <v>20161208</v>
@@ -4971,7 +4971,7 @@
     </row>
     <row r="230" spans="1:6">
       <c r="A230" s="1">
-        <v>6</v>
+        <v>228</v>
       </c>
       <c r="B230">
         <v>20161209</v>
@@ -4991,7 +4991,7 @@
     </row>
     <row r="231" spans="1:6">
       <c r="A231" s="1">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="B231">
         <v>20161212</v>
@@ -5011,7 +5011,7 @@
     </row>
     <row r="232" spans="1:6">
       <c r="A232" s="1">
-        <v>8</v>
+        <v>230</v>
       </c>
       <c r="B232">
         <v>20161213</v>
@@ -5031,7 +5031,7 @@
     </row>
     <row r="233" spans="1:6">
       <c r="A233" s="1">
-        <v>9</v>
+        <v>231</v>
       </c>
       <c r="B233">
         <v>20161214</v>
@@ -5051,7 +5051,7 @@
     </row>
     <row r="234" spans="1:6">
       <c r="A234" s="1">
-        <v>10</v>
+        <v>232</v>
       </c>
       <c r="B234">
         <v>20161215</v>
@@ -5071,7 +5071,7 @@
     </row>
     <row r="235" spans="1:6">
       <c r="A235" s="1">
-        <v>11</v>
+        <v>233</v>
       </c>
       <c r="B235">
         <v>20161216</v>
@@ -5091,7 +5091,7 @@
     </row>
     <row r="236" spans="1:6">
       <c r="A236" s="1">
-        <v>12</v>
+        <v>234</v>
       </c>
       <c r="B236">
         <v>20161219</v>
@@ -5111,7 +5111,7 @@
     </row>
     <row r="237" spans="1:6">
       <c r="A237" s="1">
-        <v>13</v>
+        <v>235</v>
       </c>
       <c r="B237">
         <v>20161220</v>
@@ -5131,7 +5131,7 @@
     </row>
     <row r="238" spans="1:6">
       <c r="A238" s="1">
-        <v>14</v>
+        <v>236</v>
       </c>
       <c r="B238">
         <v>20161221</v>
@@ -5151,7 +5151,7 @@
     </row>
     <row r="239" spans="1:6">
       <c r="A239" s="1">
-        <v>15</v>
+        <v>237</v>
       </c>
       <c r="B239">
         <v>20161222</v>
@@ -5171,7 +5171,7 @@
     </row>
     <row r="240" spans="1:6">
       <c r="A240" s="1">
-        <v>16</v>
+        <v>238</v>
       </c>
       <c r="B240">
         <v>20161223</v>
@@ -5191,7 +5191,7 @@
     </row>
     <row r="241" spans="1:6">
       <c r="A241" s="1">
-        <v>17</v>
+        <v>239</v>
       </c>
       <c r="B241">
         <v>20161226</v>
@@ -5211,7 +5211,7 @@
     </row>
     <row r="242" spans="1:6">
       <c r="A242" s="1">
-        <v>18</v>
+        <v>240</v>
       </c>
       <c r="B242">
         <v>20161227</v>
@@ -5231,7 +5231,7 @@
     </row>
     <row r="243" spans="1:6">
       <c r="A243" s="1">
-        <v>19</v>
+        <v>241</v>
       </c>
       <c r="B243">
         <v>20161228</v>
@@ -5251,7 +5251,7 @@
     </row>
     <row r="244" spans="1:6">
       <c r="A244" s="1">
-        <v>20</v>
+        <v>242</v>
       </c>
       <c r="B244">
         <v>20161229</v>
@@ -5271,7 +5271,7 @@
     </row>
     <row r="245" spans="1:6">
       <c r="A245" s="1">
-        <v>21</v>
+        <v>243</v>
       </c>
       <c r="B245">
         <v>20161230</v>

</xml_diff>